<commit_message>
added data from Kucsko 2017
</commit_message>
<xml_diff>
--- a/T2star_survey.xlsx
+++ b/T2star_survey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19284" windowHeight="3552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19284" windowHeight="3552"/>
   </bookViews>
   <sheets>
     <sheet name="T2star survey electronic spins" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="95">
   <si>
     <t>Host</t>
   </si>
@@ -568,6 +568,15 @@
   </si>
   <si>
     <t>Christle2014</t>
+  </si>
+  <si>
+    <t>55 ppm N, 45 ppm NV, 1.1% 13C</t>
+  </si>
+  <si>
+    <t>Kucsko2017</t>
+  </si>
+  <si>
+    <t>supplement 1.1, 2</t>
   </si>
 </sst>
 </file>
@@ -579,7 +588,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,8 +632,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -643,6 +660,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -656,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -666,9 +689,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,7 +720,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1017,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R27"/>
+  <dimension ref="A2:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:R20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,531 +1110,531 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>2500000000000</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>25000</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>0.05* 176000000000000000</f>
         <v>8800000000000000</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>68</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="7">
+      <c r="J3" s="4"/>
+      <c r="K3" s="6">
         <f>F3 * I3</f>
         <v>170000000000000</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <f>G3 * I3</f>
         <v>1700000</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="5" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1000000000000000</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>10000000</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f>0.75* 176000000000000000</f>
         <v>1.32E+17</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>58</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="7">
-        <f t="shared" ref="K4:K15" si="0">F4 * I4</f>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6">
+        <f t="shared" ref="K4:K16" si="0">F4 * I4</f>
         <v>5.8E+16</v>
       </c>
-      <c r="L4" s="7">
-        <f t="shared" ref="L4:L13" si="1">G4 * I4</f>
+      <c r="L4" s="6">
+        <f t="shared" ref="L4:L14" si="1">G4 * I4</f>
         <v>580000000</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="5" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1E+16</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>10000000</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>10* 176000000000000000</f>
         <v>1.76E+18</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>5</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="7">
+      <c r="J5" s="4"/>
+      <c r="K5" s="6">
         <f t="shared" si="0"/>
         <v>5E+16</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <f t="shared" si="1"/>
         <v>50000000</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="5" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f>1.7 *1.76 *100000000000000000</f>
         <v>2.992E+17</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="G6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5">
         <f>27* 176000000000000000</f>
         <v>4.752E+18</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>0.5</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="7">
+      <c r="J6" s="4"/>
+      <c r="K6" s="6">
         <f t="shared" si="0"/>
         <v>1.496E+17</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="5" t="s">
+      <c r="L6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="5" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f>0.4*1.76*100000000000000000</f>
         <v>7.0400000000000008E+16</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>10000000000</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f>0.6* 176000000000000000</f>
         <v>1.056E+17</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <f>1/3.1415/0.13</f>
         <v>2.4486098017850364</v>
       </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="7">
+      <c r="J7" s="11"/>
+      <c r="K7" s="6">
         <f t="shared" si="0"/>
         <v>1.7238213004566659E+17</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f t="shared" si="1"/>
         <v>24486098017.850365</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5" t="s">
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="5" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>50000000000</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>1</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>7000000000000000</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="7">
+      <c r="J8" s="12"/>
+      <c r="K8" s="6">
         <f t="shared" si="0"/>
         <v>925000000000</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5" t="s">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="5" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="6">
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5">
         <v>100000000000</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5">
+      <c r="H9" s="5"/>
+      <c r="I9" s="4">
         <v>0.2</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="7">
+      <c r="J9" s="4"/>
+      <c r="K9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="6">
         <f t="shared" si="1"/>
         <v>20000000000</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="5" t="s">
+      <c r="M9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5" t="s">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="5" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>7E+17</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>525000000000</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f>100* 176000000000000000</f>
         <v>1.76E+19</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>0.15</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="7">
+      <c r="J10" s="4"/>
+      <c r="K10" s="6">
         <f t="shared" si="0"/>
         <v>1.05E+17</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <f t="shared" si="1"/>
         <v>78750000000</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="O10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5" t="s">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="5" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>2.8E+18</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>218000000</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f>100* 176000000000000000</f>
         <v>1.76E+19</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>0.1</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="7">
+      <c r="J11" s="4"/>
+      <c r="K11" s="6">
         <f t="shared" si="0"/>
         <v>2.8E+17</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <f t="shared" si="1"/>
         <v>21800000</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="P11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5" t="s">
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="1" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <f>45 * 1.76 * 100000000000000000</f>
+        <v>7.92E+18</v>
+      </c>
+      <c r="G12" s="5">
+        <v>100000</v>
+      </c>
+      <c r="H12" s="4">
+        <f>55 * 1.76 * 100000000000000000</f>
+        <v>9.68E+18</v>
+      </c>
+      <c r="I12" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>4.356E+17</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="1"/>
+        <v>5500</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F13" s="13">
         <f>0.75*1.76*100000000000000000</f>
         <v>1.32E+17</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G13" s="13">
         <f>0.75*1.76*100000000000000000 *0.000000000001*10000</f>
         <v>1320000000</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="1">
+      <c r="H13" s="13"/>
+      <c r="I13" s="1">
         <v>15</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="0"/>
         <v>1.98E+18</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L13" s="6">
         <f t="shared" si="1"/>
         <v>19800000000</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="14">
-        <f>10*1.76*100000000000000000</f>
-        <v>1.7600000000000003E+18</v>
-      </c>
-      <c r="G13" s="14">
-        <f>10*1.76*100000000000000000 *0.000000000001*1000</f>
-        <v>1760000000.0000002</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7600000000000003E+18</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" si="1"/>
-        <v>1760000000.0000002</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1" t="s">
@@ -1633,480 +1653,530 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="5" t="s">
+    <row r="14" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="13">
+        <f>10*1.76*100000000000000000</f>
+        <v>1.7600000000000003E+18</v>
+      </c>
+      <c r="G14" s="13">
+        <f>10*1.76*100000000000000000 *0.000000000001*1000</f>
+        <v>1760000000.0000002</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7600000000000003E+18</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="1"/>
+        <v>1760000000.0000002</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
+      <c r="G15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" s="5" t="s">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="P15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="8" t="s">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F16" s="8">
         <v>1000000000000000</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G16" s="9">
         <v>1000000000000000</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="8">
+      <c r="H16" s="9"/>
+      <c r="I16" s="7">
         <v>1.8</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="9">
+      <c r="J16" s="7"/>
+      <c r="K16" s="8">
         <f t="shared" si="0"/>
         <v>1800000000000000</v>
       </c>
-      <c r="L15" s="9">
-        <f>G15 * I15</f>
+      <c r="L16" s="8">
+        <f>G16 * I16</f>
         <v>1800000000000000</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="O15" s="8" t="s">
+      <c r="O16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P15" s="8" t="s">
+      <c r="P16" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8" t="s">
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="5" t="s">
+    <row r="17" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5">
+      <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4">
         <v>2</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="5" t="s">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="O17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5" t="s">
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="8" t="s">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="7">
         <v>2.8E+18</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G18" s="9">
         <v>1000</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="8">
+      <c r="H18" s="9"/>
+      <c r="I18" s="7">
         <v>0.3</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="9">
-        <f t="shared" ref="K17:K19" si="2">F17 * I17</f>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8">
+        <f t="shared" ref="K18:K20" si="2">F18 * I18</f>
         <v>8.4E+17</v>
       </c>
-      <c r="L17" s="9">
-        <f>G17 * I17</f>
+      <c r="L18" s="8">
+        <f>G18 * I18</f>
         <v>300</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="N18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="O17" s="8" t="s">
+      <c r="O18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8" t="s">
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="5" t="s">
+    <row r="19" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5">
+      <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4">
         <v>1.44</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5" t="s">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="O19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5" t="s">
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="8" t="s">
+    <row r="20" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F20" s="8">
         <v>5000000000000000</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8">
+      <c r="G20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="9">
+      <c r="J20" s="7"/>
+      <c r="K20" s="8">
         <f t="shared" si="2"/>
         <v>185000000000000</v>
       </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="1" t="s">
+      <c r="L20" s="8"/>
+      <c r="M20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="N20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="O20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P19" s="8" t="s">
+      <c r="P20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8" t="s">
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="11">
+      <c r="F21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="10">
         <f>0.037/27</f>
         <v>1.3703703703703703E-3</v>
       </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5" t="s">
+      <c r="J21" s="10"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="O21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P20" s="5" t="s">
+      <c r="P21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5" t="s">
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="8" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F22" s="8">
         <v>4E+16</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1" t="s">
+      <c r="G22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="24" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="25" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="1" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1">
-        <v>120</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="2">
-        <v>120</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1">
-        <v>450</v>
+        <v>120</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="2">
-        <v>450</v>
+        <v>120</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1">
-        <v>1E-3</v>
+        <v>450</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="2">
-        <v>1E-3</v>
+        <v>450</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N26" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1">
-        <v>4</v>
+        <v>1E-3</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="2">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="28" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1">
+        <v>4</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A24:C27"/>
-    <mergeCell ref="A3:C18"/>
+    <mergeCell ref="A25:C28"/>
+    <mergeCell ref="A3:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2115,10 +2185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2182,465 +2252,465 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>2500000000000</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>25000</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>0.05* 176000000000000000</f>
         <v>8800000000000000</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>68</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7">
+      <c r="G2" s="4"/>
+      <c r="H2" s="6">
         <f>C2 * F2</f>
         <v>170000000000000</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <f>D2 * F2</f>
         <v>1700000</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1000000000000000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>10000000</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>0.75* 176000000000000000</f>
         <v>1.32E+17</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>58</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7">
-        <f t="shared" ref="H3:H14" si="0">C3 * F3</f>
+      <c r="G3" s="4"/>
+      <c r="H3" s="6">
+        <f t="shared" ref="H3:H15" si="0">C3 * F3</f>
         <v>5.8E+16</v>
       </c>
-      <c r="I3" s="7">
-        <f t="shared" ref="I3:I12" si="1">D3 * F3</f>
+      <c r="I3" s="6">
+        <f t="shared" ref="I3:I13" si="1">D3 * F3</f>
         <v>580000000</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1E+16</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>10000000</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f>10* 176000000000000000</f>
         <v>1.76E+18</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="7">
+      <c r="G4" s="4"/>
+      <c r="H4" s="6">
         <f t="shared" si="0"/>
         <v>5E+16</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <f t="shared" si="1"/>
         <v>50000000</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <f>1.7 *1.76 *100000000000000000</f>
         <v>2.992E+17</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5">
         <f>27* 176000000000000000</f>
         <v>4.752E+18</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.5</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="7">
+      <c r="G5" s="4"/>
+      <c r="H5" s="6">
         <f t="shared" si="0"/>
         <v>1.496E+17</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="I5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>0.4*1.76*100000000000000000</f>
         <v>7.0400000000000008E+16</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>10000000000</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <f>0.6* 176000000000000000</f>
         <v>1.056E+17</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <f>1/3.1415/0.13</f>
         <v>2.4486098017850364</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="7">
+      <c r="G6" s="11"/>
+      <c r="H6" s="6">
         <f t="shared" si="0"/>
         <v>1.7238213004566659E+17</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <f t="shared" si="1"/>
         <v>24486098017.850365</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>50000000000</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>7000000000000000</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="7">
+      <c r="G7" s="12"/>
+      <c r="H7" s="6">
         <f t="shared" si="0"/>
         <v>925000000000</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5" t="s">
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5">
         <v>100000000000</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5">
+      <c r="E8" s="5"/>
+      <c r="F8" s="4">
         <v>0.2</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="7">
+      <c r="G8" s="4"/>
+      <c r="H8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="6">
         <f t="shared" si="1"/>
         <v>20000000000</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="5" t="s">
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5" t="s">
+      <c r="N8" s="4"/>
+      <c r="O8" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>7E+17</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>525000000000</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f>100* 176000000000000000</f>
         <v>1.76E+19</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.15</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="7">
+      <c r="G9" s="4"/>
+      <c r="H9" s="6">
         <f t="shared" si="0"/>
         <v>1.05E+17</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
         <v>78750000000</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5" t="s">
+      <c r="N9" s="4"/>
+      <c r="O9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>2.8E+18</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>218000000</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <f>100* 176000000000000000</f>
         <v>1.76E+19</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>0.1</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="7">
+      <c r="G10" s="4"/>
+      <c r="H10" s="6">
         <f t="shared" si="0"/>
         <v>2.8E+17</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <f t="shared" si="1"/>
         <v>21800000</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="M10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5" t="s">
+      <c r="N10" s="4"/>
+      <c r="O10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="14">
-        <f>0.75*1.76*100000000000000000</f>
-        <v>1.32E+17</v>
-      </c>
-      <c r="D11" s="14">
-        <f>0.75*1.76*100000000000000000 *0.000000000001*10000</f>
-        <v>1320000000</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="1">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="C11" s="4">
+        <f>45 * 1.76 * 100000000000000000</f>
+        <v>7.92E+18</v>
+      </c>
+      <c r="D11" s="5">
+        <v>100000</v>
+      </c>
+      <c r="E11" s="4">
+        <f>55 * 1.76 * 100000000000000000</f>
+        <v>9.68E+18</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>1.98E+18</v>
-      </c>
-      <c r="I11" s="7">
+        <v>4.356E+17</v>
+      </c>
+      <c r="I11" s="6">
         <f t="shared" si="1"/>
-        <v>19800000000</v>
-      </c>
-      <c r="J11" s="1"/>
+        <v>5500</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>59</v>
+      <c r="M11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2650,28 +2720,28 @@
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="14">
-        <f>10*1.76*100000000000000000</f>
-        <v>1.7600000000000003E+18</v>
-      </c>
-      <c r="D12" s="14">
-        <f>10*1.76*100000000000000000 *0.000000000001*1000</f>
-        <v>1760000000.0000002</v>
-      </c>
-      <c r="E12" s="14"/>
+      <c r="C12" s="13">
+        <f>0.75*1.76*100000000000000000</f>
+        <v>1.32E+17</v>
+      </c>
+      <c r="D12" s="13">
+        <f>0.75*1.76*100000000000000000 *0.000000000001*10000</f>
+        <v>1320000000</v>
+      </c>
+      <c r="E12" s="13"/>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
-        <v>1.7600000000000003E+18</v>
-      </c>
-      <c r="I12" s="7">
+        <v>1.98E+18</v>
+      </c>
+      <c r="I12" s="6">
         <f t="shared" si="1"/>
-        <v>1760000000.0000002</v>
+        <v>19800000000</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
@@ -2690,272 +2760,319 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13">
+        <f>10*1.76*100000000000000000</f>
+        <v>1.7600000000000003E+18</v>
+      </c>
+      <c r="D13" s="13">
+        <f>10*1.76*100000000000000000 *0.000000000001*1000</f>
+        <v>1760000000.0000002</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7600000000000003E+18</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>1760000000.0000002</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C15" s="8">
         <v>1000000000000000</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D15" s="9">
         <v>1000000000000000</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="8">
+      <c r="E15" s="9"/>
+      <c r="F15" s="7">
         <v>1.8</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9">
+      <c r="G15" s="7"/>
+      <c r="H15" s="8">
         <f t="shared" si="0"/>
         <v>1800000000000000</v>
       </c>
-      <c r="I14" s="9">
-        <f>D14 * F14</f>
+      <c r="I15" s="8">
+        <f>D15 * F15</f>
         <v>1800000000000000</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M15" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8" t="s">
+      <c r="N15" s="7"/>
+      <c r="O15" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5">
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4">
         <v>2</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5" t="s">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C17" s="7">
         <v>2.8E+18</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D17" s="9">
         <v>1000</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="8">
+      <c r="E17" s="9"/>
+      <c r="F17" s="7">
         <v>0.3</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9">
-        <f t="shared" ref="H16:H18" si="2">C16 * F16</f>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8">
+        <f t="shared" ref="H17:H19" si="2">C17 * F17</f>
         <v>8.4E+17</v>
       </c>
-      <c r="I16" s="9">
-        <f>D16 * F16</f>
+      <c r="I17" s="8">
+        <f>D17 * F17</f>
         <v>300</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K17" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8" t="s">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5">
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
         <v>1.44</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5" t="s">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+    <row r="19" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C19" s="8">
         <v>5000000000000000</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8">
+      <c r="D19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9">
+      <c r="G19" s="7"/>
+      <c r="H19" s="8">
         <f t="shared" si="2"/>
         <v>185000000000000</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="1" t="s">
+      <c r="I19" s="8"/>
+      <c r="J19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="M19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8" t="s">
+      <c r="N19" s="7"/>
+      <c r="O19" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="11">
+      <c r="C20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="10">
         <f>0.037/27</f>
         <v>1.3703703703703703E-3</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
+      <c r="G20" s="10"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L20" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="M20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5" t="s">
+      <c r="N20" s="4"/>
+      <c r="O20" s="4" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added drawing of shaded aread to ipython
</commit_message>
<xml_diff>
--- a/T2star_survey.xlsx
+++ b/T2star_survey.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="98">
   <si>
     <t>Host</t>
   </si>
@@ -577,6 +577,16 @@
   </si>
   <si>
     <t>supplement 1.1, 2</t>
+  </si>
+  <si>
+    <t>Interrogated Vol (um^3)</t>
+  </si>
+  <si>
+    <t>Ishikawa2012
+(single NV)</t>
+  </si>
+  <si>
+    <t>20 ppm N, 45 ppm NV, 1.1% 13C</t>
   </si>
 </sst>
 </file>
@@ -679,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,6 +732,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,29 +1050,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R28"/>
+  <dimension ref="A2:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" customWidth="1"/>
-    <col min="9" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="31.21875" customWidth="1"/>
-    <col min="14" max="14" width="19.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" customWidth="1"/>
-    <col min="16" max="16" width="16.109375" customWidth="1"/>
-    <col min="17" max="17" width="36" customWidth="1"/>
-    <col min="18" max="18" width="37.77734375" customWidth="1"/>
+    <col min="6" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" customWidth="1"/>
+    <col min="10" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="31.21875" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" customWidth="1"/>
+    <col min="18" max="18" width="36" customWidth="1"/>
+    <col min="19" max="19" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1073,43 +1086,46 @@
         <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
@@ -1124,45 +1140,46 @@
       <c r="F3" s="4">
         <v>2500000000000</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5">
         <v>25000</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <f>0.05* 176000000000000000</f>
         <v>8800000000000000</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>68</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="6">
-        <f>F3 * I3</f>
+      <c r="K3" s="4"/>
+      <c r="L3" s="6">
+        <f>F3 * J3</f>
         <v>170000000000000</v>
       </c>
-      <c r="L3" s="6">
-        <f>G3 * I3</f>
+      <c r="M3" s="6">
+        <f>H3 * J3</f>
         <v>1700000</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1175,45 +1192,46 @@
       <c r="F4" s="4">
         <v>1000000000000000</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5">
         <v>10000000</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <f>0.75* 176000000000000000</f>
         <v>1.32E+17</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>58</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="6">
-        <f t="shared" ref="K4:K16" si="0">F4 * I4</f>
+      <c r="K4" s="4"/>
+      <c r="L4" s="6">
+        <f t="shared" ref="L4:L16" si="0">F4 * J4</f>
         <v>5.8E+16</v>
       </c>
-      <c r="L4" s="6">
-        <f t="shared" ref="L4:L14" si="1">G4 * I4</f>
+      <c r="M4" s="6">
+        <f t="shared" ref="M4:M14" si="1">H4 * J4</f>
         <v>580000000</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -1226,45 +1244,46 @@
       <c r="F5" s="4">
         <v>1E+16</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5">
         <v>10000000</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <f>10* 176000000000000000</f>
         <v>1.76E+18</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>5</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6">
+      <c r="K5" s="4"/>
+      <c r="L5" s="6">
         <f t="shared" si="0"/>
         <v>5E+16</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <f t="shared" si="1"/>
         <v>50000000</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -1278,40 +1297,41 @@
         <f>1.7 *1.76 *100000000000000000</f>
         <v>2.992E+17</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5">
         <f>27* 176000000000000000</f>
         <v>4.752E+18</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>0.5</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="6">
+      <c r="K6" s="4"/>
+      <c r="L6" s="6">
         <f t="shared" si="0"/>
         <v>1.496E+17</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1325,44 +1345,45 @@
         <f>0.4*1.76*100000000000000000</f>
         <v>7.0400000000000008E+16</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
         <v>10000000000</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <f>0.6* 176000000000000000</f>
         <v>1.056E+17</v>
       </c>
-      <c r="I7" s="11">
+      <c r="J7" s="11">
         <f>1/3.1415/0.13</f>
         <v>2.4486098017850364</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="6">
+      <c r="K7" s="11"/>
+      <c r="L7" s="6">
         <f t="shared" si="0"/>
         <v>1.7238213004566659E+17</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <f t="shared" si="1"/>
         <v>24486098017.850365</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -1375,42 +1396,43 @@
       <c r="F8" s="6">
         <v>50000000000</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6"/>
+      <c r="H8" s="5">
         <v>1</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>7000000000000000</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="J8" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="6">
+      <c r="K8" s="12"/>
+      <c r="L8" s="6">
         <f t="shared" si="0"/>
         <v>925000000000</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="4"/>
+      <c r="S8" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -1423,39 +1445,40 @@
       <c r="F9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4"/>
+      <c r="H9" s="5">
         <v>100000000000</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4">
+      <c r="I9" s="5"/>
+      <c r="J9" s="4">
         <v>0.2</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="6">
+      <c r="K9" s="4"/>
+      <c r="L9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="6">
         <f t="shared" si="1"/>
         <v>20000000000</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="N9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="4"/>
+      <c r="S9" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1468,43 +1491,44 @@
       <c r="F10" s="4">
         <v>7E+17</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5">
         <v>525000000000</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <f>100* 176000000000000000</f>
         <v>1.76E+19</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>0.15</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6">
+      <c r="K10" s="4"/>
+      <c r="L10" s="6">
         <f t="shared" si="0"/>
         <v>1.05E+17</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <f t="shared" si="1"/>
         <v>78750000000</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4"/>
+      <c r="S10" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -1517,43 +1541,44 @@
       <c r="F11" s="4">
         <v>2.8E+18</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4"/>
+      <c r="H11" s="5">
         <v>218000000</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <f>100* 176000000000000000</f>
         <v>1.76E+19</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>0.1</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="6">
+      <c r="K11" s="4"/>
+      <c r="L11" s="6">
         <f t="shared" si="0"/>
         <v>2.8E+17</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M11" s="6">
         <f t="shared" si="1"/>
         <v>21800000</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4"/>
+      <c r="S11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -1567,43 +1592,44 @@
         <f>45 * 1.76 * 100000000000000000</f>
         <v>7.92E+18</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4"/>
+      <c r="H12" s="5">
         <v>100000</v>
       </c>
-      <c r="H12" s="4">
-        <f>55 * 1.76 * 100000000000000000</f>
-        <v>9.68E+18</v>
-      </c>
       <c r="I12" s="4">
+        <f>20 * 1.76 * 100000000000000000</f>
+        <v>3.5200000000000005E+18</v>
+      </c>
+      <c r="J12" s="4">
         <v>5.5E-2</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="6">
+      <c r="K12" s="4"/>
+      <c r="L12" s="6">
         <f t="shared" si="0"/>
         <v>4.356E+17</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
         <f t="shared" si="1"/>
         <v>5500</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="P12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4"/>
+      <c r="S12" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1617,43 +1643,44 @@
         <f>0.75*1.76*100000000000000000</f>
         <v>1.32E+17</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
         <f>0.75*1.76*100000000000000000 *0.000000000001*10000</f>
         <v>1320000000</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="1">
+      <c r="I13" s="13"/>
+      <c r="J13" s="1">
         <v>15</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="K13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="1">
         <f t="shared" si="0"/>
         <v>1.98E+18</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <f t="shared" si="1"/>
         <v>19800000000</v>
       </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="1"/>
+      <c r="O13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1667,43 +1694,44 @@
         <f>10*1.76*100000000000000000</f>
         <v>1.7600000000000003E+18</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13">
         <f>10*1.76*100000000000000000 *0.000000000001*1000</f>
         <v>1760000000.0000002</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="1">
+      <c r="I14" s="13"/>
+      <c r="J14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="1">
+      <c r="K14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="1">
         <f t="shared" si="0"/>
         <v>1.7600000000000003E+18</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="6">
         <f t="shared" si="1"/>
         <v>1760000000.0000002</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1" t="s">
+      <c r="N14" s="1"/>
+      <c r="O14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1716,34 +1744,35 @@
       <c r="F15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="L15" s="4"/>
       <c r="M15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1756,40 +1785,41 @@
       <c r="F16" s="8">
         <v>1000000000000000</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8"/>
+      <c r="H16" s="9">
         <v>1000000000000000</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="7">
+      <c r="I16" s="9"/>
+      <c r="J16" s="7">
         <v>1.8</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8">
+      <c r="K16" s="7"/>
+      <c r="L16" s="8">
         <f t="shared" si="0"/>
         <v>1800000000000000</v>
       </c>
-      <c r="L16" s="8">
-        <f>G16 * I16</f>
+      <c r="M16" s="8">
+        <f>H16 * J16</f>
         <v>1800000000000000</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="N16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="O16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="O16" s="7" t="s">
+      <c r="P16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P16" s="7" t="s">
+      <c r="Q16" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7" t="s">
+      <c r="R16" s="7"/>
+      <c r="S16" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -1802,34 +1832,35 @@
       <c r="F17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
         <v>2</v>
       </c>
-      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="L17" s="4"/>
       <c r="M17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="O17" s="4" t="s">
+      <c r="P17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R17" s="4"/>
-    </row>
-    <row r="18" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1842,38 +1873,39 @@
       <c r="F18" s="7">
         <v>2.8E+18</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7"/>
+      <c r="H18" s="9">
         <v>1000</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="7">
+      <c r="I18" s="9"/>
+      <c r="J18" s="7">
         <v>0.3</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="8">
-        <f t="shared" ref="K18:K20" si="2">F18 * I18</f>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8">
+        <f t="shared" ref="L18:L20" si="2">F18 * J18</f>
         <v>8.4E+17</v>
       </c>
-      <c r="L18" s="8">
-        <f>G18 * I18</f>
+      <c r="M18" s="8">
+        <f>H18 * J18</f>
         <v>300</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="O18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="P18" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="7" t="s">
+      <c r="R18" s="7"/>
+      <c r="S18" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -1886,32 +1918,33 @@
       <c r="F19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4">
         <v>1.44</v>
       </c>
-      <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="O19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O19" s="4" t="s">
+      <c r="P19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1924,37 +1957,38 @@
       <c r="F20" s="8">
         <v>5000000000000000</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7">
+      <c r="G20" s="8"/>
+      <c r="H20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="8">
+      <c r="K20" s="7"/>
+      <c r="L20" s="8">
         <f t="shared" si="2"/>
         <v>185000000000000</v>
       </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="8"/>
+      <c r="N20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="7" t="s">
+      <c r="O20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="O20" s="7" t="s">
+      <c r="P20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P20" s="7" t="s">
+      <c r="Q20" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7" t="s">
+      <c r="R20" s="7"/>
+      <c r="S20" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -1967,33 +2001,34 @@
       <c r="F21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="10">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="10">
         <f>0.037/27</f>
         <v>1.3703703703703703E-3</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="4"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="4" t="s">
+      <c r="N21" s="4"/>
+      <c r="O21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="P21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P21" s="4" t="s">
+      <c r="Q21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="4"/>
+      <c r="S21" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2006,26 +2041,27 @@
       <c r="F22" s="8">
         <v>4E+16</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="1"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="7"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="1" t="s">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-    </row>
-    <row r="25" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="S22" s="1"/>
+    </row>
+    <row r="25" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>36</v>
       </c>
@@ -2040,31 +2076,32 @@
       <c r="F25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
         <v>120</v>
       </c>
-      <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="2">
+      <c r="L25" s="1"/>
+      <c r="M25" s="2">
         <v>120</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -2077,31 +2114,32 @@
       <c r="F26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1">
         <v>450</v>
       </c>
-      <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="2">
+      <c r="L26" s="1"/>
+      <c r="M26" s="2">
         <v>450</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -2114,29 +2152,30 @@
       <c r="F27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1">
         <v>1E-3</v>
       </c>
-      <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="2">
+      <c r="L27" s="1"/>
+      <c r="M27" s="2">
         <v>1E-3</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2149,27 +2188,28 @@
       <c r="F28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
         <v>4</v>
       </c>
-      <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="2">
+      <c r="L28" s="1"/>
+      <c r="M28" s="2">
         <v>1</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>